<commit_message>
Updated TC3 for multiplicative
</commit_message>
<xml_diff>
--- a/Test Case - 2/TC2_Results_B.xlsx
+++ b/Test Case - 2/TC2_Results_B.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="outfile" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="115">
   <si>
     <t>56ad1cbb-a42b-4fcf-bd5d-e16a2513146b</t>
   </si>
@@ -120,9 +120,6 @@
     <t>3ddd035f-50bb-4175-bb94-a5ba570bab4d</t>
   </si>
   <si>
-    <t>7bfc64c9-67f3-4021-9602-09b7ecb860db</t>
-  </si>
-  <si>
     <t>05f71dc2-8eb5-417a-8f3a-ae2d0e187dbf</t>
   </si>
   <si>
@@ -141,9 +138,6 @@
     <t>8db23287-6de0-4ef9-b0e7-bb86bb25fa42</t>
   </si>
   <si>
-    <t>f5065a9c-1e3b-4e85-93bd-6a2becd653cc</t>
-  </si>
-  <si>
     <t>f1f620e2-c8c5-48ab-a5ff-08c14e7d75f6</t>
   </si>
   <si>
@@ -151,9 +145,6 @@
   </si>
   <si>
     <t>d7da79fc-4e63-4489-b797-78c843c46b0c</t>
-  </si>
-  <si>
-    <t>e9ceeb89-50a0-4dff-bdd4-3335313a5a30</t>
   </si>
   <si>
     <t>8bf64e93-e47b-4660-83d6-88b2625da1a0</t>
@@ -860,13 +851,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -916,7 +907,68 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1192,101 +1244,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T105"/>
+  <dimension ref="A1:T103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3:O45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="T1" s="3"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="T1" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="4" t="s">
+      <c r="E2" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="R2" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="T2" s="4"/>
+      <c r="G2" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="T2" s="3"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -1342,6 +1392,10 @@
       </c>
       <c r="R3">
         <v>35.152000000000001</v>
+      </c>
+      <c r="T3">
+        <f>IF(K3=TRUE,1,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -1399,6 +1453,10 @@
       <c r="R4">
         <v>35.152000000000001</v>
       </c>
+      <c r="T4">
+        <f t="shared" ref="T4:T67" si="0">IF(K4=TRUE,1,0)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -1455,6 +1513,10 @@
       <c r="R5">
         <v>35.152000000000001</v>
       </c>
+      <c r="T5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1511,6 +1573,10 @@
       <c r="R6">
         <v>35.152000000000001</v>
       </c>
+      <c r="T6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1567,6 +1633,10 @@
       <c r="R7">
         <v>35.152000000000001</v>
       </c>
+      <c r="T7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1623,6 +1693,10 @@
       <c r="R8">
         <v>35.152000000000001</v>
       </c>
+      <c r="T8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -1679,6 +1753,10 @@
       <c r="R9">
         <v>35.152000000000001</v>
       </c>
+      <c r="T9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1735,6 +1813,10 @@
       <c r="R10">
         <v>35.152000000000001</v>
       </c>
+      <c r="T10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1791,6 +1873,10 @@
       <c r="R11">
         <v>35.152000000000001</v>
       </c>
+      <c r="T11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1847,6 +1933,10 @@
       <c r="R12">
         <v>35.152000000000001</v>
       </c>
+      <c r="T12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1903,6 +1993,10 @@
       <c r="R13">
         <v>35.152000000000001</v>
       </c>
+      <c r="T13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1959,6 +2053,10 @@
       <c r="R14">
         <v>35.152000000000001</v>
       </c>
+      <c r="T14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -2015,6 +2113,10 @@
       <c r="R15">
         <v>35.152000000000001</v>
       </c>
+      <c r="T15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -2071,8 +2173,12 @@
       <c r="R16">
         <v>35.152000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2127,8 +2233,12 @@
       <c r="R17">
         <v>35.152000000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2183,8 +2293,12 @@
       <c r="R18">
         <v>35.152000000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2239,8 +2353,12 @@
       <c r="R19">
         <v>35.152000000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2295,8 +2413,12 @@
       <c r="R20">
         <v>35.152000000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T20">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2351,8 +2473,12 @@
       <c r="R21">
         <v>35.152000000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2407,8 +2533,12 @@
       <c r="R22">
         <v>35.152000000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2463,8 +2593,12 @@
       <c r="R23">
         <v>35.152000000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2519,8 +2653,12 @@
       <c r="R24">
         <v>35.152000000000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2575,8 +2713,12 @@
       <c r="R25">
         <v>35.152000000000001</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2631,8 +2773,12 @@
       <c r="R26">
         <v>35.152000000000001</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T26">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2687,8 +2833,12 @@
       <c r="R27">
         <v>35.152000000000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T27">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2743,8 +2893,12 @@
       <c r="R28">
         <v>35.152000000000001</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2799,8 +2953,12 @@
       <c r="R29">
         <v>35.152000000000001</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2855,8 +3013,12 @@
       <c r="R30">
         <v>35.152000000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2911,8 +3073,12 @@
       <c r="R31">
         <v>35.152000000000001</v>
       </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2967,8 +3133,12 @@
       <c r="R32">
         <v>35.152000000000001</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -3023,8 +3193,12 @@
       <c r="R33">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -3079,8 +3253,12 @@
       <c r="R34">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -3135,22 +3313,26 @@
       <c r="R35">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B36">
-        <v>30.132000000000001</v>
+        <v>28.488</v>
       </c>
       <c r="C36">
-        <v>52.238</v>
+        <v>54.686999999999998</v>
       </c>
       <c r="D36">
         <v>35.152000000000001</v>
       </c>
       <c r="E36">
-        <v>31.545084970000001</v>
+        <v>28.454915029999999</v>
       </c>
       <c r="F36">
         <v>54.755282579999999</v>
@@ -3165,42 +3347,55 @@
         <v>6.3005460270000002</v>
       </c>
       <c r="J36">
-        <v>0</v>
+        <v>6.3709168975074997</v>
       </c>
       <c r="K36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L36">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N36">
         <v>1</v>
       </c>
       <c r="O36" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="P36">
+        <v>26.931999999999999</v>
+      </c>
+      <c r="Q36">
+        <v>39.482999999999997</v>
+      </c>
+      <c r="R36">
+        <v>40.152000000000001</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B37">
-        <v>28.488</v>
+        <v>25.952999999999999</v>
       </c>
       <c r="C37">
-        <v>54.686999999999998</v>
+        <v>52.87</v>
       </c>
       <c r="D37">
         <v>35.152000000000001</v>
       </c>
       <c r="E37">
-        <v>28.454915029999999</v>
+        <v>25.954915029999999</v>
       </c>
       <c r="F37">
-        <v>54.755282579999999</v>
+        <v>52.938926260000002</v>
       </c>
       <c r="G37">
         <v>35</v>
@@ -3238,25 +3433,29 @@
       <c r="R37">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T37">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B38">
-        <v>25.952999999999999</v>
+        <v>25.015999999999998</v>
       </c>
       <c r="C38">
-        <v>52.87</v>
+        <v>49.95</v>
       </c>
       <c r="D38">
         <v>35.152000000000001</v>
       </c>
       <c r="E38">
-        <v>25.954915029999999</v>
+        <v>25</v>
       </c>
       <c r="F38">
-        <v>52.938926260000002</v>
+        <v>50</v>
       </c>
       <c r="G38">
         <v>35</v>
@@ -3294,25 +3493,29 @@
       <c r="R38">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B39">
-        <v>25.015999999999998</v>
+        <v>25.988</v>
       </c>
       <c r="C39">
-        <v>49.95</v>
+        <v>46.993000000000002</v>
       </c>
       <c r="D39">
         <v>35.152000000000001</v>
       </c>
       <c r="E39">
-        <v>25</v>
+        <v>25.954915029999999</v>
       </c>
       <c r="F39">
-        <v>50</v>
+        <v>47.061073739999998</v>
       </c>
       <c r="G39">
         <v>35</v>
@@ -3333,10 +3536,10 @@
         <v>94</v>
       </c>
       <c r="M39">
-        <v>1</v>
+        <v>1.0070517258695999</v>
       </c>
       <c r="N39">
-        <v>1</v>
+        <v>1.0051237500000001</v>
       </c>
       <c r="O39" t="b">
         <v>1</v>
@@ -3350,25 +3553,29 @@
       <c r="R39">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T39">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B40">
-        <v>25.988</v>
+        <v>28.452999999999999</v>
       </c>
       <c r="C40">
-        <v>46.993000000000002</v>
+        <v>45.194000000000003</v>
       </c>
       <c r="D40">
         <v>35.152000000000001</v>
       </c>
       <c r="E40">
-        <v>25.954915029999999</v>
+        <v>28.454915029999999</v>
       </c>
       <c r="F40">
-        <v>47.061073739999998</v>
+        <v>45.244717420000001</v>
       </c>
       <c r="G40">
         <v>35</v>
@@ -3389,10 +3596,10 @@
         <v>94</v>
       </c>
       <c r="M40">
-        <v>1.0070517258695999</v>
+        <v>1.09814507380868</v>
       </c>
       <c r="N40">
-        <v>1.0051237500000001</v>
+        <v>1.09629143</v>
       </c>
       <c r="O40" t="b">
         <v>1</v>
@@ -3406,22 +3613,26 @@
       <c r="R40">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T40">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B41">
-        <v>28.452999999999999</v>
+        <v>31.577999999999999</v>
       </c>
       <c r="C41">
-        <v>45.194000000000003</v>
+        <v>45.177</v>
       </c>
       <c r="D41">
         <v>35.152000000000001</v>
       </c>
       <c r="E41">
-        <v>28.454915029999999</v>
+        <v>31.545084970000001</v>
       </c>
       <c r="F41">
         <v>45.244717420000001</v>
@@ -3442,10 +3653,10 @@
         <v>1</v>
       </c>
       <c r="L41">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M41">
-        <v>1.09814507380868</v>
+        <v>1.09833945558263</v>
       </c>
       <c r="N41">
         <v>1.09629143</v>
@@ -3454,33 +3665,37 @@
         <v>1</v>
       </c>
       <c r="P41">
-        <v>26.931999999999999</v>
+        <v>33.121000000000002</v>
       </c>
       <c r="Q41">
-        <v>39.482999999999997</v>
+        <v>39.475000000000001</v>
       </c>
       <c r="R41">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T41">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B42">
-        <v>31.577999999999999</v>
+        <v>34.042999999999999</v>
       </c>
       <c r="C42">
-        <v>45.177</v>
+        <v>47.011000000000003</v>
       </c>
       <c r="D42">
         <v>35.152000000000001</v>
       </c>
       <c r="E42">
-        <v>31.545084970000001</v>
+        <v>34.045084969999998</v>
       </c>
       <c r="F42">
-        <v>45.244717420000001</v>
+        <v>47.061073739999998</v>
       </c>
       <c r="G42">
         <v>35</v>
@@ -3501,10 +3716,10 @@
         <v>93</v>
       </c>
       <c r="M42">
-        <v>1.09833945558263</v>
+        <v>1.00597849527914</v>
       </c>
       <c r="N42">
-        <v>1.09629143</v>
+        <v>1.0051237500000001</v>
       </c>
       <c r="O42" t="b">
         <v>1</v>
@@ -3518,25 +3733,29 @@
       <c r="R42">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B43">
-        <v>31.664999999999999</v>
+        <v>54.997999999999998</v>
       </c>
       <c r="C43">
-        <v>47.539000000000001</v>
+        <v>39.966999999999999</v>
       </c>
       <c r="D43">
         <v>35.152000000000001</v>
       </c>
       <c r="E43">
-        <v>31.545084970000001</v>
+        <v>55</v>
       </c>
       <c r="F43">
-        <v>45.244717420000001</v>
+        <v>40</v>
       </c>
       <c r="G43">
         <v>35</v>
@@ -3548,42 +3767,55 @@
         <v>6.3005460270000002</v>
       </c>
       <c r="J43">
-        <v>0</v>
+        <v>6.5958920135495802</v>
       </c>
       <c r="K43" t="b">
         <v>0</v>
       </c>
       <c r="L43">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M43">
+        <v>1</v>
+      </c>
+      <c r="N43">
+        <v>1</v>
+      </c>
+      <c r="O43" t="b">
+        <v>1</v>
+      </c>
+      <c r="P43">
+        <v>38.121000000000002</v>
+      </c>
+      <c r="Q43">
+        <v>35.834000000000003</v>
+      </c>
+      <c r="R43">
+        <v>40.152000000000001</v>
+      </c>
+      <c r="T43">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N43">
-        <v>1.09629143</v>
-      </c>
-      <c r="O43" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B44">
-        <v>34.042999999999999</v>
+        <v>54.061</v>
       </c>
       <c r="C44">
-        <v>47.011000000000003</v>
+        <v>42.889000000000003</v>
       </c>
       <c r="D44">
         <v>35.152000000000001</v>
       </c>
       <c r="E44">
-        <v>34.045084969999998</v>
+        <v>54.045084969999998</v>
       </c>
       <c r="F44">
-        <v>47.061073739999998</v>
+        <v>42.938926260000002</v>
       </c>
       <c r="G44">
         <v>35</v>
@@ -3595,57 +3827,61 @@
         <v>6.3005460270000002</v>
       </c>
       <c r="J44">
-        <v>6.3709168975074997</v>
+        <v>6.5958920135495802</v>
       </c>
       <c r="K44" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L44">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M44">
-        <v>1.00597849527914</v>
+        <v>1</v>
       </c>
       <c r="N44">
-        <v>1.0051237500000001</v>
+        <v>1</v>
       </c>
       <c r="O44" t="b">
         <v>1</v>
       </c>
       <c r="P44">
-        <v>33.121000000000002</v>
+        <v>38.121000000000002</v>
       </c>
       <c r="Q44">
-        <v>39.475000000000001</v>
+        <v>35.834000000000003</v>
       </c>
       <c r="R44">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T44">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B45">
-        <v>54.997999999999998</v>
+        <v>54.061</v>
       </c>
       <c r="C45">
-        <v>39.966999999999999</v>
+        <v>42.889000000000003</v>
       </c>
       <c r="D45">
         <v>35.152000000000001</v>
       </c>
       <c r="E45">
-        <v>55</v>
+        <v>51.545084969999998</v>
       </c>
       <c r="F45">
-        <v>40</v>
+        <v>44.755282579999999</v>
       </c>
       <c r="G45">
         <v>35</v>
       </c>
       <c r="H45" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I45">
         <v>6.3005460270000002</v>
@@ -3677,78 +3913,35 @@
       <c r="R45">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>42</v>
-      </c>
-      <c r="B46">
-        <v>54.061</v>
-      </c>
-      <c r="C46">
-        <v>42.889000000000003</v>
-      </c>
-      <c r="D46">
-        <v>35.152000000000001</v>
-      </c>
-      <c r="E46">
-        <v>54.045084969999998</v>
-      </c>
-      <c r="F46">
-        <v>42.938926260000002</v>
-      </c>
-      <c r="G46">
-        <v>35</v>
-      </c>
-      <c r="H46" t="s">
-        <v>43</v>
-      </c>
-      <c r="I46">
-        <v>6.3005460270000002</v>
-      </c>
-      <c r="J46">
-        <v>6.5958920135495802</v>
-      </c>
-      <c r="K46" t="b">
+        <v>44</v>
+      </c>
+      <c r="T46">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L46">
-        <v>92</v>
-      </c>
-      <c r="M46">
-        <v>1</v>
-      </c>
-      <c r="N46">
-        <v>1</v>
-      </c>
-      <c r="O46" t="b">
-        <v>1</v>
-      </c>
-      <c r="P46">
-        <v>38.121000000000002</v>
-      </c>
-      <c r="Q46">
-        <v>35.834000000000003</v>
-      </c>
-      <c r="R46">
-        <v>40.152000000000001</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B47">
-        <v>52.311</v>
+        <v>45.97</v>
       </c>
       <c r="C47">
-        <v>41.508000000000003</v>
+        <v>42.905999999999999</v>
       </c>
       <c r="D47">
         <v>35.152000000000001</v>
       </c>
       <c r="E47">
-        <v>54.045084969999998</v>
+        <v>45.954915030000002</v>
       </c>
       <c r="F47">
         <v>42.938926260000002</v>
@@ -3757,13 +3950,13 @@
         <v>35</v>
       </c>
       <c r="H47" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I47">
         <v>6.3005460270000002</v>
       </c>
       <c r="J47">
-        <v>0</v>
+        <v>6.5958920135495802</v>
       </c>
       <c r="K47" t="b">
         <v>0</v>
@@ -3772,33 +3965,46 @@
         <v>92</v>
       </c>
       <c r="M47">
+        <v>1</v>
+      </c>
+      <c r="N47">
+        <v>1</v>
+      </c>
+      <c r="O47" t="b">
+        <v>1</v>
+      </c>
+      <c r="P47">
+        <v>38.121000000000002</v>
+      </c>
+      <c r="Q47">
+        <v>35.834000000000003</v>
+      </c>
+      <c r="R47">
+        <v>40.152000000000001</v>
+      </c>
+      <c r="T47">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N47">
-        <v>1</v>
-      </c>
-      <c r="O47" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B48">
-        <v>54.061</v>
+        <v>44.997999999999998</v>
       </c>
       <c r="C48">
-        <v>42.889000000000003</v>
+        <v>39.932000000000002</v>
       </c>
       <c r="D48">
         <v>35.152000000000001</v>
       </c>
       <c r="E48">
-        <v>51.545084969999998</v>
+        <v>45</v>
       </c>
       <c r="F48">
-        <v>44.755282579999999</v>
+        <v>40</v>
       </c>
       <c r="G48">
         <v>35</v>
@@ -3836,16 +4042,20 @@
       <c r="R48">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B49">
-        <v>45.97</v>
+        <v>45.988</v>
       </c>
       <c r="C49">
-        <v>42.905999999999999</v>
+        <v>36.993000000000002</v>
       </c>
       <c r="D49">
         <v>35.152000000000001</v>
@@ -3854,13 +4064,13 @@
         <v>45.954915030000002</v>
       </c>
       <c r="F49">
-        <v>42.938926260000002</v>
+        <v>37.061073739999998</v>
       </c>
       <c r="G49">
         <v>35</v>
       </c>
       <c r="H49" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I49">
         <v>6.3005460270000002</v>
@@ -3892,31 +4102,35 @@
       <c r="R49">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B50">
-        <v>44.997999999999998</v>
+        <v>48.488</v>
       </c>
       <c r="C50">
-        <v>39.932000000000002</v>
+        <v>35.194000000000003</v>
       </c>
       <c r="D50">
         <v>35.152000000000001</v>
       </c>
       <c r="E50">
-        <v>45</v>
+        <v>48.454915030000002</v>
       </c>
       <c r="F50">
-        <v>40</v>
+        <v>35.244717420000001</v>
       </c>
       <c r="G50">
         <v>35</v>
       </c>
       <c r="H50" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I50">
         <v>6.3005460270000002</v>
@@ -3928,7 +4142,7 @@
         <v>0</v>
       </c>
       <c r="L50">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M50">
         <v>1</v>
@@ -3940,39 +4154,43 @@
         <v>1</v>
       </c>
       <c r="P50">
-        <v>38.121000000000002</v>
+        <v>40.023000000000003</v>
       </c>
       <c r="Q50">
-        <v>35.834000000000003</v>
+        <v>29.957000000000001</v>
       </c>
       <c r="R50">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T50">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B51">
-        <v>45.988</v>
+        <v>51.542999999999999</v>
       </c>
       <c r="C51">
-        <v>36.993000000000002</v>
+        <v>35.194000000000003</v>
       </c>
       <c r="D51">
         <v>35.152000000000001</v>
       </c>
       <c r="E51">
-        <v>45.954915030000002</v>
+        <v>51.545084969999998</v>
       </c>
       <c r="F51">
-        <v>37.061073739999998</v>
+        <v>35.244717420000001</v>
       </c>
       <c r="G51">
         <v>35</v>
       </c>
       <c r="H51" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I51">
         <v>6.3005460270000002</v>
@@ -3984,7 +4202,7 @@
         <v>0</v>
       </c>
       <c r="L51">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M51">
         <v>1</v>
@@ -3996,39 +4214,43 @@
         <v>1</v>
       </c>
       <c r="P51">
-        <v>38.121000000000002</v>
+        <v>40.023000000000003</v>
       </c>
       <c r="Q51">
-        <v>35.834000000000003</v>
+        <v>29.957000000000001</v>
       </c>
       <c r="R51">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B52">
-        <v>48.488</v>
+        <v>54.042999999999999</v>
       </c>
       <c r="C52">
-        <v>35.194000000000003</v>
+        <v>37.027999999999999</v>
       </c>
       <c r="D52">
         <v>35.152000000000001</v>
       </c>
       <c r="E52">
-        <v>48.454915030000002</v>
+        <v>54.045084969999998</v>
       </c>
       <c r="F52">
-        <v>35.244717420000001</v>
+        <v>37.061073739999998</v>
       </c>
       <c r="G52">
         <v>35</v>
       </c>
       <c r="H52" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I52">
         <v>6.3005460270000002</v>
@@ -4060,43 +4282,47 @@
       <c r="R52">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T52">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B53">
-        <v>51.542999999999999</v>
+        <v>55.033000000000001</v>
       </c>
       <c r="C53">
-        <v>35.194000000000003</v>
+        <v>19.95</v>
       </c>
       <c r="D53">
         <v>35.152000000000001</v>
       </c>
       <c r="E53">
-        <v>51.545084969999998</v>
+        <v>55</v>
       </c>
       <c r="F53">
-        <v>35.244717420000001</v>
+        <v>20</v>
       </c>
       <c r="G53">
         <v>35</v>
       </c>
       <c r="H53" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I53">
         <v>6.3005460270000002</v>
       </c>
       <c r="J53">
-        <v>6.5958920135495802</v>
+        <v>6.3732216262409001</v>
       </c>
       <c r="K53" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L53">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="M53">
         <v>1</v>
@@ -4108,48 +4334,52 @@
         <v>1</v>
       </c>
       <c r="P53">
-        <v>40.023000000000003</v>
+        <v>38.121000000000002</v>
       </c>
       <c r="Q53">
-        <v>29.957000000000001</v>
+        <v>24.071000000000002</v>
       </c>
       <c r="R53">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T53">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B54">
-        <v>54.042999999999999</v>
+        <v>54.043999999999997</v>
       </c>
       <c r="C54">
-        <v>37.027999999999999</v>
+        <v>22.904</v>
       </c>
       <c r="D54">
         <v>35.152000000000001</v>
       </c>
       <c r="E54">
-        <v>51.545084969999998</v>
+        <v>54.045084969999998</v>
       </c>
       <c r="F54">
-        <v>35.244717420000001</v>
+        <v>22.938926259999999</v>
       </c>
       <c r="G54">
         <v>35</v>
       </c>
       <c r="H54" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I54">
         <v>6.3005460270000002</v>
       </c>
       <c r="J54">
-        <v>6.5958920135495802</v>
+        <v>6.3732216262409001</v>
       </c>
       <c r="K54" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L54">
         <v>91</v>
@@ -4172,25 +4402,29 @@
       <c r="R54">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T54">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B55">
-        <v>54.042999999999999</v>
+        <v>51.576999999999998</v>
       </c>
       <c r="C55">
-        <v>37.027999999999999</v>
+        <v>24.687999999999999</v>
       </c>
       <c r="D55">
         <v>35.152000000000001</v>
       </c>
       <c r="E55">
-        <v>54.045084969999998</v>
+        <v>51.545084969999998</v>
       </c>
       <c r="F55">
-        <v>37.061073739999998</v>
+        <v>24.755282579999999</v>
       </c>
       <c r="G55">
         <v>35</v>
@@ -4202,7 +4436,7 @@
         <v>6.3005460270000002</v>
       </c>
       <c r="J55">
-        <v>6.5958920135495802</v>
+        <v>0</v>
       </c>
       <c r="K55" t="b">
         <v>0</v>
@@ -4211,42 +4445,37 @@
         <v>91</v>
       </c>
       <c r="M55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N55">
         <v>1</v>
       </c>
       <c r="O55" t="b">
-        <v>1</v>
-      </c>
-      <c r="P55">
-        <v>40.023000000000003</v>
-      </c>
-      <c r="Q55">
-        <v>29.957000000000001</v>
-      </c>
-      <c r="R55">
-        <v>40.152000000000001</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="T55">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B56">
-        <v>55.033000000000001</v>
+        <v>48.487000000000002</v>
       </c>
       <c r="C56">
-        <v>19.95</v>
+        <v>24.704000000000001</v>
       </c>
       <c r="D56">
         <v>35.152000000000001</v>
       </c>
       <c r="E56">
-        <v>55</v>
+        <v>48.454915030000002</v>
       </c>
       <c r="F56">
-        <v>20</v>
+        <v>24.755282579999999</v>
       </c>
       <c r="G56">
         <v>35</v>
@@ -4264,7 +4493,7 @@
         <v>1</v>
       </c>
       <c r="L56">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="M56">
         <v>1</v>
@@ -4276,21 +4505,25 @@
         <v>1</v>
       </c>
       <c r="P56">
-        <v>38.121000000000002</v>
+        <v>40.023000000000003</v>
       </c>
       <c r="Q56">
-        <v>24.071000000000002</v>
+        <v>29.957000000000001</v>
       </c>
       <c r="R56">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T56">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B57">
-        <v>54.043999999999997</v>
+        <v>45.954000000000001</v>
       </c>
       <c r="C57">
         <v>22.904</v>
@@ -4299,7 +4532,7 @@
         <v>35.152000000000001</v>
       </c>
       <c r="E57">
-        <v>54.045084969999998</v>
+        <v>45.954915030000002</v>
       </c>
       <c r="F57">
         <v>22.938926259999999</v>
@@ -4320,7 +4553,7 @@
         <v>1</v>
       </c>
       <c r="L57">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="M57">
         <v>1</v>
@@ -4332,33 +4565,37 @@
         <v>1</v>
       </c>
       <c r="P57">
-        <v>40.023000000000003</v>
+        <v>38.121000000000002</v>
       </c>
       <c r="Q57">
-        <v>29.957000000000001</v>
+        <v>24.071000000000002</v>
       </c>
       <c r="R57">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T57">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B58">
-        <v>51.576999999999998</v>
+        <v>45.015000000000001</v>
       </c>
       <c r="C58">
-        <v>24.687999999999999</v>
+        <v>19.981999999999999</v>
       </c>
       <c r="D58">
         <v>35.152000000000001</v>
       </c>
       <c r="E58">
-        <v>51.545084969999998</v>
+        <v>45</v>
       </c>
       <c r="F58">
-        <v>24.755282579999999</v>
+        <v>20</v>
       </c>
       <c r="G58">
         <v>35</v>
@@ -4370,42 +4607,55 @@
         <v>6.3005460270000002</v>
       </c>
       <c r="J58">
-        <v>0</v>
+        <v>6.3732216262409001</v>
       </c>
       <c r="K58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L58">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="M58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N58">
         <v>1</v>
       </c>
       <c r="O58" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="P58">
+        <v>38.121000000000002</v>
+      </c>
+      <c r="Q58">
+        <v>24.071000000000002</v>
+      </c>
+      <c r="R58">
+        <v>40.152000000000001</v>
+      </c>
+      <c r="T58">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B59">
-        <v>48.487000000000002</v>
+        <v>46.003</v>
       </c>
       <c r="C59">
-        <v>24.704000000000001</v>
+        <v>17.010000000000002</v>
       </c>
       <c r="D59">
         <v>35.152000000000001</v>
       </c>
       <c r="E59">
-        <v>48.454915030000002</v>
+        <v>45.954915030000002</v>
       </c>
       <c r="F59">
-        <v>24.755282579999999</v>
+        <v>17.061073740000001</v>
       </c>
       <c r="G59">
         <v>35</v>
@@ -4423,7 +4673,7 @@
         <v>1</v>
       </c>
       <c r="L59">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="M59">
         <v>1</v>
@@ -4435,33 +4685,37 @@
         <v>1</v>
       </c>
       <c r="P59">
-        <v>40.023000000000003</v>
+        <v>38.121000000000002</v>
       </c>
       <c r="Q59">
-        <v>29.957000000000001</v>
+        <v>24.071000000000002</v>
       </c>
       <c r="R59">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T59">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B60">
-        <v>45.954000000000001</v>
+        <v>48.47</v>
       </c>
       <c r="C60">
-        <v>22.904</v>
+        <v>15.194000000000001</v>
       </c>
       <c r="D60">
         <v>35.152000000000001</v>
       </c>
       <c r="E60">
-        <v>45.954915030000002</v>
+        <v>48.454915030000002</v>
       </c>
       <c r="F60">
-        <v>22.938926259999999</v>
+        <v>15.244717420000001</v>
       </c>
       <c r="G60">
         <v>35</v>
@@ -4499,25 +4753,29 @@
       <c r="R60">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T60">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B61">
-        <v>45.015000000000001</v>
+        <v>51.56</v>
       </c>
       <c r="C61">
-        <v>19.981999999999999</v>
+        <v>15.21</v>
       </c>
       <c r="D61">
         <v>35.152000000000001</v>
       </c>
       <c r="E61">
-        <v>45</v>
+        <v>51.545084969999998</v>
       </c>
       <c r="F61">
-        <v>20</v>
+        <v>15.244717420000001</v>
       </c>
       <c r="G61">
         <v>35</v>
@@ -4555,22 +4813,26 @@
       <c r="R61">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T61">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B62">
-        <v>46.003</v>
+        <v>54.043999999999997</v>
       </c>
       <c r="C62">
-        <v>17.010000000000002</v>
+        <v>17.044</v>
       </c>
       <c r="D62">
         <v>35.152000000000001</v>
       </c>
       <c r="E62">
-        <v>45.954915030000002</v>
+        <v>54.045084969999998</v>
       </c>
       <c r="F62">
         <v>17.061073740000001</v>
@@ -4611,25 +4873,29 @@
       <c r="R62">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T62">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B63">
-        <v>48.47</v>
+        <v>35.015000000000001</v>
       </c>
       <c r="C63">
-        <v>15.194000000000001</v>
+        <v>10.015000000000001</v>
       </c>
       <c r="D63">
         <v>35.152000000000001</v>
       </c>
       <c r="E63">
-        <v>48.454915030000002</v>
+        <v>35</v>
       </c>
       <c r="F63">
-        <v>15.244717420000001</v>
+        <v>10</v>
       </c>
       <c r="G63">
         <v>35</v>
@@ -4641,13 +4907,13 @@
         <v>6.3005460270000002</v>
       </c>
       <c r="J63">
-        <v>6.3732216262409001</v>
+        <v>6.3688731277536696</v>
       </c>
       <c r="K63" t="b">
         <v>1</v>
       </c>
       <c r="L63">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M63">
         <v>1</v>
@@ -4659,33 +4925,37 @@
         <v>1</v>
       </c>
       <c r="P63">
-        <v>38.121000000000002</v>
+        <v>33.121000000000002</v>
       </c>
       <c r="Q63">
-        <v>24.071000000000002</v>
+        <v>20.43</v>
       </c>
       <c r="R63">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T63">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B64">
-        <v>51.56</v>
+        <v>34.06</v>
       </c>
       <c r="C64">
-        <v>15.21</v>
+        <v>12.888</v>
       </c>
       <c r="D64">
         <v>35.152000000000001</v>
       </c>
       <c r="E64">
-        <v>51.545084969999998</v>
+        <v>34.045084969999998</v>
       </c>
       <c r="F64">
-        <v>15.244717420000001</v>
+        <v>12.938926260000001</v>
       </c>
       <c r="G64">
         <v>35</v>
@@ -4697,51 +4967,55 @@
         <v>6.3005460270000002</v>
       </c>
       <c r="J64">
-        <v>6.3732216262409001</v>
+        <v>6.3688731277536696</v>
       </c>
       <c r="K64" t="b">
         <v>1</v>
       </c>
       <c r="L64">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M64">
-        <v>1</v>
+        <v>1.0056060299759799</v>
       </c>
       <c r="N64">
-        <v>1</v>
+        <v>1.0051237500000001</v>
       </c>
       <c r="O64" t="b">
         <v>1</v>
       </c>
       <c r="P64">
-        <v>38.121000000000002</v>
+        <v>33.121000000000002</v>
       </c>
       <c r="Q64">
-        <v>24.071000000000002</v>
+        <v>20.43</v>
       </c>
       <c r="R64">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T64">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B65">
-        <v>54.043999999999997</v>
+        <v>31.544</v>
       </c>
       <c r="C65">
-        <v>17.044</v>
+        <v>14.721</v>
       </c>
       <c r="D65">
         <v>35.152000000000001</v>
       </c>
       <c r="E65">
-        <v>54.045084969999998</v>
+        <v>31.545084970000001</v>
       </c>
       <c r="F65">
-        <v>17.061073740000001</v>
+        <v>14.755282579999999</v>
       </c>
       <c r="G65">
         <v>35</v>
@@ -4753,51 +5027,55 @@
         <v>6.3005460270000002</v>
       </c>
       <c r="J65">
-        <v>6.3732216262409001</v>
+        <v>6.3688731277536696</v>
       </c>
       <c r="K65" t="b">
         <v>1</v>
       </c>
       <c r="L65">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="M65">
-        <v>1</v>
+        <v>1.0973183183908599</v>
       </c>
       <c r="N65">
-        <v>1</v>
+        <v>1.09629143</v>
       </c>
       <c r="O65" t="b">
         <v>1</v>
       </c>
       <c r="P65">
-        <v>38.121000000000002</v>
+        <v>33.121000000000002</v>
       </c>
       <c r="Q65">
-        <v>24.071000000000002</v>
+        <v>20.43</v>
       </c>
       <c r="R65">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T65">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B66">
-        <v>35.015000000000001</v>
+        <v>28.47</v>
       </c>
       <c r="C66">
-        <v>10.015000000000001</v>
+        <v>14.738</v>
       </c>
       <c r="D66">
         <v>35.152000000000001</v>
       </c>
       <c r="E66">
-        <v>35</v>
+        <v>28.454915029999999</v>
       </c>
       <c r="F66">
-        <v>10</v>
+        <v>14.755282579999999</v>
       </c>
       <c r="G66">
         <v>35</v>
@@ -4815,42 +5093,46 @@
         <v>1</v>
       </c>
       <c r="L66">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M66">
-        <v>1</v>
+        <v>1.0985500628677101</v>
       </c>
       <c r="N66">
-        <v>1</v>
+        <v>1.09629143</v>
       </c>
       <c r="O66" t="b">
         <v>1</v>
       </c>
       <c r="P66">
-        <v>33.121000000000002</v>
+        <v>26.931999999999999</v>
       </c>
       <c r="Q66">
-        <v>20.43</v>
+        <v>20.437999999999999</v>
       </c>
       <c r="R66">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T66">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B67">
-        <v>34.06</v>
+        <v>25.97</v>
       </c>
       <c r="C67">
-        <v>12.888</v>
+        <v>12.904</v>
       </c>
       <c r="D67">
         <v>35.152000000000001</v>
       </c>
       <c r="E67">
-        <v>34.045084969999998</v>
+        <v>25.954915029999999</v>
       </c>
       <c r="F67">
         <v>12.938926260000001</v>
@@ -4871,10 +5153,10 @@
         <v>1</v>
       </c>
       <c r="L67">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M67">
-        <v>1.0056060299759799</v>
+        <v>1.0058404495940401</v>
       </c>
       <c r="N67">
         <v>1.0051237500000001</v>
@@ -4883,33 +5165,37 @@
         <v>1</v>
       </c>
       <c r="P67">
-        <v>33.121000000000002</v>
+        <v>26.931999999999999</v>
       </c>
       <c r="Q67">
-        <v>20.43</v>
+        <v>20.437999999999999</v>
       </c>
       <c r="R67">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T67">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B68">
-        <v>31.544</v>
+        <v>24.998999999999999</v>
       </c>
       <c r="C68">
-        <v>14.721</v>
+        <v>9.9489999999999998</v>
       </c>
       <c r="D68">
         <v>35.152000000000001</v>
       </c>
       <c r="E68">
-        <v>31.545084970000001</v>
+        <v>25</v>
       </c>
       <c r="F68">
-        <v>14.755282579999999</v>
+        <v>10</v>
       </c>
       <c r="G68">
         <v>35</v>
@@ -4927,45 +5213,49 @@
         <v>1</v>
       </c>
       <c r="L68">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M68">
-        <v>1.0973183183908599</v>
+        <v>1</v>
       </c>
       <c r="N68">
-        <v>1.09629143</v>
+        <v>1</v>
       </c>
       <c r="O68" t="b">
         <v>1</v>
       </c>
       <c r="P68">
-        <v>33.121000000000002</v>
+        <v>26.931999999999999</v>
       </c>
       <c r="Q68">
-        <v>20.43</v>
+        <v>20.437999999999999</v>
       </c>
       <c r="R68">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T68">
+        <f t="shared" ref="T68:T102" si="1">IF(K68=TRUE,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B69">
-        <v>28.47</v>
+        <v>25.97</v>
       </c>
       <c r="C69">
-        <v>14.738</v>
+        <v>7.0259999999999998</v>
       </c>
       <c r="D69">
         <v>35.152000000000001</v>
       </c>
       <c r="E69">
-        <v>28.454915029999999</v>
+        <v>25.954915029999999</v>
       </c>
       <c r="F69">
-        <v>14.755282579999999</v>
+        <v>7.0610737390000002</v>
       </c>
       <c r="G69">
         <v>35</v>
@@ -4986,10 +5276,10 @@
         <v>98</v>
       </c>
       <c r="M69">
-        <v>1.0985500628677101</v>
+        <v>1</v>
       </c>
       <c r="N69">
-        <v>1.09629143</v>
+        <v>1</v>
       </c>
       <c r="O69" t="b">
         <v>1</v>
@@ -5003,25 +5293,29 @@
       <c r="R69">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T69">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B70">
-        <v>25.97</v>
+        <v>28.47</v>
       </c>
       <c r="C70">
-        <v>12.904</v>
+        <v>5.194</v>
       </c>
       <c r="D70">
         <v>35.152000000000001</v>
       </c>
       <c r="E70">
-        <v>25.954915029999999</v>
+        <v>28.454915029999999</v>
       </c>
       <c r="F70">
-        <v>12.938926260000001</v>
+        <v>5.2447174189999997</v>
       </c>
       <c r="G70">
         <v>35</v>
@@ -5042,10 +5336,10 @@
         <v>98</v>
       </c>
       <c r="M70">
-        <v>1.0058404495940401</v>
+        <v>1</v>
       </c>
       <c r="N70">
-        <v>1.0051237500000001</v>
+        <v>1</v>
       </c>
       <c r="O70" t="b">
         <v>1</v>
@@ -5059,25 +5353,29 @@
       <c r="R70">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T70">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B71">
-        <v>24.998999999999999</v>
+        <v>31.56</v>
       </c>
       <c r="C71">
-        <v>9.9489999999999998</v>
+        <v>5.194</v>
       </c>
       <c r="D71">
         <v>35.152000000000001</v>
       </c>
       <c r="E71">
-        <v>25</v>
+        <v>31.545084970000001</v>
       </c>
       <c r="F71">
-        <v>10</v>
+        <v>5.2447174189999997</v>
       </c>
       <c r="G71">
         <v>35</v>
@@ -5095,7 +5393,7 @@
         <v>1</v>
       </c>
       <c r="L71">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="M71">
         <v>1</v>
@@ -5107,21 +5405,25 @@
         <v>1</v>
       </c>
       <c r="P71">
-        <v>26.931999999999999</v>
+        <v>33.121000000000002</v>
       </c>
       <c r="Q71">
-        <v>20.437999999999999</v>
+        <v>20.43</v>
       </c>
       <c r="R71">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T71">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B72">
-        <v>25.97</v>
+        <v>34.043999999999997</v>
       </c>
       <c r="C72">
         <v>7.0259999999999998</v>
@@ -5130,7 +5432,7 @@
         <v>35.152000000000001</v>
       </c>
       <c r="E72">
-        <v>25.954915029999999</v>
+        <v>34.045084969999998</v>
       </c>
       <c r="F72">
         <v>7.0610737390000002</v>
@@ -5151,7 +5453,7 @@
         <v>1</v>
       </c>
       <c r="L72">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="M72">
         <v>1</v>
@@ -5163,33 +5465,37 @@
         <v>1</v>
       </c>
       <c r="P72">
-        <v>26.931999999999999</v>
+        <v>33.121000000000002</v>
       </c>
       <c r="Q72">
-        <v>20.437999999999999</v>
+        <v>20.43</v>
       </c>
       <c r="R72">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T72">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B73">
-        <v>28.47</v>
+        <v>15.015000000000001</v>
       </c>
       <c r="C73">
-        <v>5.194</v>
+        <v>19.949000000000002</v>
       </c>
       <c r="D73">
         <v>35.152000000000001</v>
       </c>
       <c r="E73">
-        <v>28.454915029999999</v>
+        <v>15</v>
       </c>
       <c r="F73">
-        <v>5.2447174189999997</v>
+        <v>20</v>
       </c>
       <c r="G73">
         <v>35</v>
@@ -5201,13 +5507,13 @@
         <v>6.3005460270000002</v>
       </c>
       <c r="J73">
-        <v>6.3688731277536696</v>
+        <v>6.3697667319368696</v>
       </c>
       <c r="K73" t="b">
         <v>1</v>
       </c>
       <c r="L73">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M73">
         <v>1</v>
@@ -5219,33 +5525,37 @@
         <v>1</v>
       </c>
       <c r="P73">
-        <v>26.931999999999999</v>
+        <v>21.925000000000001</v>
       </c>
       <c r="Q73">
-        <v>20.437999999999999</v>
+        <v>24.087</v>
       </c>
       <c r="R73">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T73">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B74">
-        <v>31.56</v>
+        <v>14.06</v>
       </c>
       <c r="C74">
-        <v>5.194</v>
+        <v>22.920999999999999</v>
       </c>
       <c r="D74">
         <v>35.152000000000001</v>
       </c>
       <c r="E74">
-        <v>31.545084970000001</v>
+        <v>14.04508497</v>
       </c>
       <c r="F74">
-        <v>5.2447174189999997</v>
+        <v>22.938926259999999</v>
       </c>
       <c r="G74">
         <v>35</v>
@@ -5257,13 +5567,13 @@
         <v>6.3005460270000002</v>
       </c>
       <c r="J74">
-        <v>6.3688731277536696</v>
+        <v>6.3697667319368696</v>
       </c>
       <c r="K74" t="b">
         <v>1</v>
       </c>
       <c r="L74">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="M74">
         <v>1</v>
@@ -5275,33 +5585,37 @@
         <v>1</v>
       </c>
       <c r="P74">
-        <v>33.121000000000002</v>
+        <v>21.925000000000001</v>
       </c>
       <c r="Q74">
-        <v>20.43</v>
+        <v>24.087</v>
       </c>
       <c r="R74">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T74">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B75">
-        <v>34.043999999999997</v>
+        <v>11.56</v>
       </c>
       <c r="C75">
-        <v>7.0259999999999998</v>
+        <v>24.721</v>
       </c>
       <c r="D75">
         <v>35.152000000000001</v>
       </c>
       <c r="E75">
-        <v>34.045084969999998</v>
+        <v>11.54508497</v>
       </c>
       <c r="F75">
-        <v>7.0610737390000002</v>
+        <v>24.755282579999999</v>
       </c>
       <c r="G75">
         <v>35</v>
@@ -5313,13 +5627,13 @@
         <v>6.3005460270000002</v>
       </c>
       <c r="J75">
-        <v>6.3688731277536696</v>
+        <v>6.3697667319368696</v>
       </c>
       <c r="K75" t="b">
         <v>1</v>
       </c>
       <c r="L75">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="M75">
         <v>1</v>
@@ -5331,33 +5645,37 @@
         <v>1</v>
       </c>
       <c r="P75">
-        <v>33.121000000000002</v>
+        <v>20.015000000000001</v>
       </c>
       <c r="Q75">
-        <v>20.43</v>
+        <v>29.963999999999999</v>
       </c>
       <c r="R75">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T75">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B76">
-        <v>15.015000000000001</v>
+        <v>8.4870000000000001</v>
       </c>
       <c r="C76">
-        <v>19.949000000000002</v>
+        <v>24.721</v>
       </c>
       <c r="D76">
         <v>35.152000000000001</v>
       </c>
       <c r="E76">
-        <v>15</v>
+        <v>8.4549150280000003</v>
       </c>
       <c r="F76">
-        <v>20</v>
+        <v>24.755282579999999</v>
       </c>
       <c r="G76">
         <v>35</v>
@@ -5375,7 +5693,7 @@
         <v>1</v>
       </c>
       <c r="L76">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M76">
         <v>1</v>
@@ -5387,30 +5705,34 @@
         <v>1</v>
       </c>
       <c r="P76">
-        <v>21.925000000000001</v>
+        <v>20.015000000000001</v>
       </c>
       <c r="Q76">
-        <v>24.087</v>
+        <v>29.963999999999999</v>
       </c>
       <c r="R76">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T76">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B77">
-        <v>14.06</v>
+        <v>5.9539999999999997</v>
       </c>
       <c r="C77">
-        <v>22.920999999999999</v>
+        <v>22.872</v>
       </c>
       <c r="D77">
         <v>35.152000000000001</v>
       </c>
       <c r="E77">
-        <v>14.04508497</v>
+        <v>5.9549150280000003</v>
       </c>
       <c r="F77">
         <v>22.938926259999999</v>
@@ -5431,7 +5753,7 @@
         <v>1</v>
       </c>
       <c r="L77">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M77">
         <v>1</v>
@@ -5443,33 +5765,37 @@
         <v>1</v>
       </c>
       <c r="P77">
-        <v>21.925000000000001</v>
+        <v>20.015000000000001</v>
       </c>
       <c r="Q77">
-        <v>24.087</v>
+        <v>29.963999999999999</v>
       </c>
       <c r="R77">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T77">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B78">
-        <v>11.56</v>
+        <v>5.0149999999999997</v>
       </c>
       <c r="C78">
-        <v>24.721</v>
+        <v>19.933</v>
       </c>
       <c r="D78">
         <v>35.152000000000001</v>
       </c>
       <c r="E78">
-        <v>11.54508497</v>
+        <v>5</v>
       </c>
       <c r="F78">
-        <v>24.755282579999999</v>
+        <v>20</v>
       </c>
       <c r="G78">
         <v>35</v>
@@ -5487,7 +5813,7 @@
         <v>1</v>
       </c>
       <c r="L78">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M78">
         <v>1</v>
@@ -5499,33 +5825,37 @@
         <v>1</v>
       </c>
       <c r="P78">
-        <v>20.015000000000001</v>
+        <v>21.925000000000001</v>
       </c>
       <c r="Q78">
-        <v>29.963999999999999</v>
+        <v>24.087</v>
       </c>
       <c r="R78">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T78">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B79">
-        <v>8.4870000000000001</v>
+        <v>5.9880000000000004</v>
       </c>
       <c r="C79">
-        <v>24.721</v>
+        <v>16.992999999999999</v>
       </c>
       <c r="D79">
         <v>35.152000000000001</v>
       </c>
       <c r="E79">
-        <v>8.4549150280000003</v>
+        <v>5.9549150280000003</v>
       </c>
       <c r="F79">
-        <v>24.755282579999999</v>
+        <v>17.061073740000001</v>
       </c>
       <c r="G79">
         <v>35</v>
@@ -5543,7 +5873,7 @@
         <v>1</v>
       </c>
       <c r="L79">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M79">
         <v>1</v>
@@ -5555,33 +5885,37 @@
         <v>1</v>
       </c>
       <c r="P79">
-        <v>20.015000000000001</v>
+        <v>21.925000000000001</v>
       </c>
       <c r="Q79">
-        <v>29.963999999999999</v>
+        <v>24.087</v>
       </c>
       <c r="R79">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T79">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B80">
-        <v>5.9539999999999997</v>
+        <v>8.48</v>
       </c>
       <c r="C80">
-        <v>22.872</v>
+        <v>15.183999999999999</v>
       </c>
       <c r="D80">
         <v>35.152000000000001</v>
       </c>
       <c r="E80">
-        <v>5.9549150280000003</v>
+        <v>8.4549150280000003</v>
       </c>
       <c r="F80">
-        <v>22.938926259999999</v>
+        <v>15.244717420000001</v>
       </c>
       <c r="G80">
         <v>35</v>
@@ -5599,7 +5933,7 @@
         <v>1</v>
       </c>
       <c r="L80">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M80">
         <v>1</v>
@@ -5611,33 +5945,37 @@
         <v>1</v>
       </c>
       <c r="P80">
-        <v>20.015000000000001</v>
+        <v>21.925000000000001</v>
       </c>
       <c r="Q80">
-        <v>29.963999999999999</v>
+        <v>24.087</v>
       </c>
       <c r="R80">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T80">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B81">
-        <v>5.0149999999999997</v>
+        <v>11.571</v>
       </c>
       <c r="C81">
-        <v>19.933</v>
+        <v>15.201000000000001</v>
       </c>
       <c r="D81">
         <v>35.152000000000001</v>
       </c>
       <c r="E81">
-        <v>5</v>
+        <v>11.54508497</v>
       </c>
       <c r="F81">
-        <v>20</v>
+        <v>15.244717420000001</v>
       </c>
       <c r="G81">
         <v>35</v>
@@ -5675,22 +6013,26 @@
       <c r="R81">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T81">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B82">
-        <v>5.9880000000000004</v>
+        <v>14.061999999999999</v>
       </c>
       <c r="C82">
-        <v>16.992999999999999</v>
+        <v>17.026</v>
       </c>
       <c r="D82">
         <v>35.152000000000001</v>
       </c>
       <c r="E82">
-        <v>5.9549150280000003</v>
+        <v>14.04508497</v>
       </c>
       <c r="F82">
         <v>17.061073740000001</v>
@@ -5731,25 +6073,29 @@
       <c r="R82">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T82">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B83">
-        <v>8.48</v>
+        <v>15.032999999999999</v>
       </c>
       <c r="C83">
-        <v>15.183999999999999</v>
+        <v>39.947000000000003</v>
       </c>
       <c r="D83">
         <v>35.152000000000001</v>
       </c>
       <c r="E83">
-        <v>8.4549150280000003</v>
+        <v>15</v>
       </c>
       <c r="F83">
-        <v>15.244717420000001</v>
+        <v>40</v>
       </c>
       <c r="G83">
         <v>35</v>
@@ -5761,13 +6107,13 @@
         <v>6.3005460270000002</v>
       </c>
       <c r="J83">
-        <v>6.3697667319368696</v>
+        <v>6.3720684871527498</v>
       </c>
       <c r="K83" t="b">
         <v>1</v>
       </c>
       <c r="L83">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="M83">
         <v>1</v>
@@ -5779,33 +6125,37 @@
         <v>1</v>
       </c>
       <c r="P83">
-        <v>21.925000000000001</v>
+        <v>21.940999999999999</v>
       </c>
       <c r="Q83">
-        <v>24.087</v>
+        <v>35.834000000000003</v>
       </c>
       <c r="R83">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T83">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B84">
-        <v>11.571</v>
+        <v>14.07</v>
       </c>
       <c r="C84">
-        <v>15.201000000000001</v>
+        <v>42.902999999999999</v>
       </c>
       <c r="D84">
         <v>35.152000000000001</v>
       </c>
       <c r="E84">
-        <v>11.54508497</v>
+        <v>14.04508497</v>
       </c>
       <c r="F84">
-        <v>15.244717420000001</v>
+        <v>42.938926260000002</v>
       </c>
       <c r="G84">
         <v>35</v>
@@ -5817,13 +6167,13 @@
         <v>6.3005460270000002</v>
       </c>
       <c r="J84">
-        <v>6.3697667319368696</v>
+        <v>6.3720684871527498</v>
       </c>
       <c r="K84" t="b">
         <v>1</v>
       </c>
       <c r="L84">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="M84">
         <v>1</v>
@@ -5835,33 +6185,37 @@
         <v>1</v>
       </c>
       <c r="P84">
-        <v>21.925000000000001</v>
+        <v>21.940999999999999</v>
       </c>
       <c r="Q84">
-        <v>24.087</v>
+        <v>35.834000000000003</v>
       </c>
       <c r="R84">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T84">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B85">
-        <v>14.061999999999999</v>
+        <v>11.569000000000001</v>
       </c>
       <c r="C85">
-        <v>17.026</v>
+        <v>44.712000000000003</v>
       </c>
       <c r="D85">
         <v>35.152000000000001</v>
       </c>
       <c r="E85">
-        <v>14.04508497</v>
+        <v>11.54508497</v>
       </c>
       <c r="F85">
-        <v>17.061073740000001</v>
+        <v>44.755282579999999</v>
       </c>
       <c r="G85">
         <v>35</v>
@@ -5873,13 +6227,13 @@
         <v>6.3005460270000002</v>
       </c>
       <c r="J85">
-        <v>6.3697667319368696</v>
+        <v>6.3720684871527498</v>
       </c>
       <c r="K85" t="b">
         <v>1</v>
       </c>
       <c r="L85">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="M85">
         <v>1</v>
@@ -5891,33 +6245,37 @@
         <v>1</v>
       </c>
       <c r="P85">
-        <v>21.925000000000001</v>
+        <v>21.940999999999999</v>
       </c>
       <c r="Q85">
-        <v>24.087</v>
+        <v>35.834000000000003</v>
       </c>
       <c r="R85">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T85">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B86">
-        <v>15.032999999999999</v>
+        <v>8.4779999999999998</v>
       </c>
       <c r="C86">
-        <v>39.947000000000003</v>
+        <v>44.704000000000001</v>
       </c>
       <c r="D86">
         <v>35.152000000000001</v>
       </c>
       <c r="E86">
-        <v>15</v>
+        <v>8.4549150280000003</v>
       </c>
       <c r="F86">
-        <v>40</v>
+        <v>44.755282579999999</v>
       </c>
       <c r="G86">
         <v>35</v>
@@ -5955,22 +6313,26 @@
       <c r="R86">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T86">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B87">
-        <v>14.07</v>
+        <v>5.9779999999999998</v>
       </c>
       <c r="C87">
-        <v>42.902999999999999</v>
+        <v>42.887</v>
       </c>
       <c r="D87">
         <v>35.152000000000001</v>
       </c>
       <c r="E87">
-        <v>14.04508497</v>
+        <v>5.9549150280000003</v>
       </c>
       <c r="F87">
         <v>42.938926260000002</v>
@@ -6011,25 +6373,29 @@
       <c r="R87">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T87">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B88">
-        <v>11.569000000000001</v>
+        <v>5.0309999999999997</v>
       </c>
       <c r="C88">
-        <v>44.712000000000003</v>
+        <v>39.957000000000001</v>
       </c>
       <c r="D88">
         <v>35.152000000000001</v>
       </c>
       <c r="E88">
-        <v>11.54508497</v>
+        <v>5</v>
       </c>
       <c r="F88">
-        <v>44.755282579999999</v>
+        <v>40</v>
       </c>
       <c r="G88">
         <v>35</v>
@@ -6067,25 +6433,29 @@
       <c r="R88">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T88">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B89">
-        <v>8.4779999999999998</v>
+        <v>5.9859999999999998</v>
       </c>
       <c r="C89">
-        <v>44.704000000000001</v>
+        <v>37.018000000000001</v>
       </c>
       <c r="D89">
         <v>35.152000000000001</v>
       </c>
       <c r="E89">
-        <v>8.4549150280000003</v>
+        <v>5.9549150280000003</v>
       </c>
       <c r="F89">
-        <v>44.755282579999999</v>
+        <v>37.061073739999998</v>
       </c>
       <c r="G89">
         <v>35</v>
@@ -6103,7 +6473,7 @@
         <v>1</v>
       </c>
       <c r="L89">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M89">
         <v>1</v>
@@ -6115,33 +6485,37 @@
         <v>1</v>
       </c>
       <c r="P89">
-        <v>21.940999999999999</v>
+        <v>20.015000000000001</v>
       </c>
       <c r="Q89">
-        <v>35.834000000000003</v>
+        <v>29.963999999999999</v>
       </c>
       <c r="R89">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T89">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B90">
-        <v>5.9779999999999998</v>
+        <v>8.4779999999999998</v>
       </c>
       <c r="C90">
-        <v>42.887</v>
+        <v>35.201000000000001</v>
       </c>
       <c r="D90">
         <v>35.152000000000001</v>
       </c>
       <c r="E90">
-        <v>5.9549150280000003</v>
+        <v>8.4549150280000003</v>
       </c>
       <c r="F90">
-        <v>42.938926260000002</v>
+        <v>35.244717420000001</v>
       </c>
       <c r="G90">
         <v>35</v>
@@ -6159,7 +6533,7 @@
         <v>1</v>
       </c>
       <c r="L90">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M90">
         <v>1</v>
@@ -6171,33 +6545,37 @@
         <v>1</v>
       </c>
       <c r="P90">
-        <v>21.940999999999999</v>
+        <v>20.015000000000001</v>
       </c>
       <c r="Q90">
-        <v>35.834000000000003</v>
+        <v>29.963999999999999</v>
       </c>
       <c r="R90">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T90">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B91">
-        <v>5.0309999999999997</v>
+        <v>11.569000000000001</v>
       </c>
       <c r="C91">
-        <v>39.957000000000001</v>
+        <v>35.192999999999998</v>
       </c>
       <c r="D91">
         <v>35.152000000000001</v>
       </c>
       <c r="E91">
-        <v>5</v>
+        <v>11.54508497</v>
       </c>
       <c r="F91">
-        <v>40</v>
+        <v>35.244717420000001</v>
       </c>
       <c r="G91">
         <v>35</v>
@@ -6215,7 +6593,7 @@
         <v>1</v>
       </c>
       <c r="L91">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M91">
         <v>1</v>
@@ -6227,21 +6605,25 @@
         <v>1</v>
       </c>
       <c r="P91">
-        <v>21.940999999999999</v>
+        <v>20.015000000000001</v>
       </c>
       <c r="Q91">
-        <v>35.834000000000003</v>
+        <v>29.963999999999999</v>
       </c>
       <c r="R91">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T91">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B92">
-        <v>5.9859999999999998</v>
+        <v>14.068</v>
       </c>
       <c r="C92">
         <v>37.018000000000001</v>
@@ -6250,7 +6632,7 @@
         <v>35.152000000000001</v>
       </c>
       <c r="E92">
-        <v>5.9549150280000003</v>
+        <v>14.04508497</v>
       </c>
       <c r="F92">
         <v>37.061073739999998</v>
@@ -6271,7 +6653,7 @@
         <v>1</v>
       </c>
       <c r="L92">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M92">
         <v>1</v>
@@ -6283,52 +6665,53 @@
         <v>1</v>
       </c>
       <c r="P92">
-        <v>20.015000000000001</v>
+        <v>21.940999999999999</v>
       </c>
       <c r="Q92">
-        <v>29.963999999999999</v>
+        <v>35.834000000000003</v>
       </c>
       <c r="R92">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T92">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B93">
-        <v>8.4779999999999998</v>
+        <v>40.023000000000003</v>
       </c>
       <c r="C93">
-        <v>35.201000000000001</v>
+        <v>29.957000000000001</v>
       </c>
       <c r="D93">
-        <v>35.152000000000001</v>
+        <v>40.152000000000001</v>
       </c>
       <c r="E93">
-        <v>8.4549150280000003</v>
+        <v>40</v>
       </c>
       <c r="F93">
-        <v>35.244717420000001</v>
+        <v>30</v>
       </c>
       <c r="G93">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H93" t="s">
         <v>88</v>
       </c>
       <c r="I93">
-        <v>6.3005460270000002</v>
+        <v>7.7283896780000001</v>
       </c>
       <c r="J93">
-        <v>6.3720684871527498</v>
+        <v>7.73638277602298</v>
       </c>
       <c r="K93" t="b">
         <v>1</v>
       </c>
-      <c r="L93">
-        <v>96</v>
-      </c>
       <c r="M93">
         <v>1</v>
       </c>
@@ -6338,53 +6721,45 @@
       <c r="O93" t="b">
         <v>1</v>
       </c>
-      <c r="P93">
-        <v>20.015000000000001</v>
-      </c>
-      <c r="Q93">
-        <v>29.963999999999999</v>
-      </c>
-      <c r="R93">
+      <c r="T93">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>92</v>
+      </c>
+      <c r="B94">
+        <v>38.121000000000002</v>
+      </c>
+      <c r="C94">
+        <v>35.834000000000003</v>
+      </c>
+      <c r="D94">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A94">
-        <v>89</v>
-      </c>
-      <c r="B94">
-        <v>11.569000000000001</v>
-      </c>
-      <c r="C94">
-        <v>35.192999999999998</v>
-      </c>
-      <c r="D94">
-        <v>35.152000000000001</v>
-      </c>
       <c r="E94">
-        <v>11.54508497</v>
+        <v>38.090169940000003</v>
       </c>
       <c r="F94">
-        <v>35.244717420000001</v>
+        <v>35.877852519999998</v>
       </c>
       <c r="G94">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H94" t="s">
         <v>89</v>
       </c>
       <c r="I94">
-        <v>6.3005460270000002</v>
+        <v>7.7283896780000001</v>
       </c>
       <c r="J94">
-        <v>6.3720684871527498</v>
+        <v>7.73638277602298</v>
       </c>
       <c r="K94" t="b">
         <v>1</v>
       </c>
-      <c r="L94">
-        <v>96</v>
-      </c>
       <c r="M94">
         <v>1</v>
       </c>
@@ -6394,53 +6769,45 @@
       <c r="O94" t="b">
         <v>1</v>
       </c>
-      <c r="P94">
-        <v>20.015000000000001</v>
-      </c>
-      <c r="Q94">
-        <v>29.963999999999999</v>
-      </c>
-      <c r="R94">
+      <c r="T94">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>93</v>
+      </c>
+      <c r="B95">
+        <v>33.121000000000002</v>
+      </c>
+      <c r="C95">
+        <v>39.475000000000001</v>
+      </c>
+      <c r="D95">
         <v>40.152000000000001</v>
       </c>
-    </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A95">
-        <v>90</v>
-      </c>
-      <c r="B95">
-        <v>14.068</v>
-      </c>
-      <c r="C95">
-        <v>37.018000000000001</v>
-      </c>
-      <c r="D95">
-        <v>35.152000000000001</v>
-      </c>
       <c r="E95">
-        <v>14.04508497</v>
+        <v>33.090169940000003</v>
       </c>
       <c r="F95">
-        <v>37.061073739999998</v>
+        <v>39.510565159999999</v>
       </c>
       <c r="G95">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H95" t="s">
         <v>90</v>
       </c>
       <c r="I95">
-        <v>6.3005460270000002</v>
+        <v>7.7283896780000001</v>
       </c>
       <c r="J95">
-        <v>6.3720684871527498</v>
+        <v>7.73638277602298</v>
       </c>
       <c r="K95" t="b">
         <v>1</v>
       </c>
-      <c r="L95">
-        <v>95</v>
-      </c>
       <c r="M95">
         <v>1</v>
       </c>
@@ -6450,34 +6817,29 @@
       <c r="O95" t="b">
         <v>1</v>
       </c>
-      <c r="P95">
-        <v>21.940999999999999</v>
-      </c>
-      <c r="Q95">
-        <v>35.834000000000003</v>
-      </c>
-      <c r="R95">
-        <v>40.152000000000001</v>
-      </c>
-    </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="T95">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B96">
-        <v>40.023000000000003</v>
+        <v>26.931999999999999</v>
       </c>
       <c r="C96">
-        <v>29.957000000000001</v>
+        <v>39.482999999999997</v>
       </c>
       <c r="D96">
         <v>40.152000000000001</v>
       </c>
       <c r="E96">
-        <v>40</v>
+        <v>26.909830060000001</v>
       </c>
       <c r="F96">
-        <v>30</v>
+        <v>39.510565159999999</v>
       </c>
       <c r="G96">
         <v>40</v>
@@ -6503,13 +6865,17 @@
       <c r="O96" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="T96">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B97">
-        <v>38.121000000000002</v>
+        <v>21.940999999999999</v>
       </c>
       <c r="C97">
         <v>35.834000000000003</v>
@@ -6518,7 +6884,7 @@
         <v>40.152000000000001</v>
       </c>
       <c r="E97">
-        <v>38.090169940000003</v>
+        <v>21.909830060000001</v>
       </c>
       <c r="F97">
         <v>35.877852519999998</v>
@@ -6547,25 +6913,29 @@
       <c r="O97" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="T97">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B98">
-        <v>33.121000000000002</v>
+        <v>20.015000000000001</v>
       </c>
       <c r="C98">
-        <v>39.475000000000001</v>
+        <v>29.963999999999999</v>
       </c>
       <c r="D98">
         <v>40.152000000000001</v>
       </c>
       <c r="E98">
-        <v>33.090169940000003</v>
+        <v>20</v>
       </c>
       <c r="F98">
-        <v>39.510565159999999</v>
+        <v>30</v>
       </c>
       <c r="G98">
         <v>40</v>
@@ -6591,25 +6961,29 @@
       <c r="O98" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="T98">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B99">
-        <v>26.931999999999999</v>
+        <v>21.925000000000001</v>
       </c>
       <c r="C99">
-        <v>39.482999999999997</v>
+        <v>24.087</v>
       </c>
       <c r="D99">
         <v>40.152000000000001</v>
       </c>
       <c r="E99">
-        <v>26.909830060000001</v>
+        <v>21.909830060000001</v>
       </c>
       <c r="F99">
-        <v>39.510565159999999</v>
+        <v>24.122147479999999</v>
       </c>
       <c r="G99">
         <v>40</v>
@@ -6635,25 +7009,29 @@
       <c r="O99" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="T99">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B100">
-        <v>21.940999999999999</v>
+        <v>26.931999999999999</v>
       </c>
       <c r="C100">
-        <v>35.834000000000003</v>
+        <v>20.437999999999999</v>
       </c>
       <c r="D100">
         <v>40.152000000000001</v>
       </c>
       <c r="E100">
-        <v>21.909830060000001</v>
+        <v>26.909830060000001</v>
       </c>
       <c r="F100">
-        <v>35.877852519999998</v>
+        <v>20.489434840000001</v>
       </c>
       <c r="G100">
         <v>40</v>
@@ -6679,25 +7057,29 @@
       <c r="O100" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="T100">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B101">
-        <v>20.015000000000001</v>
+        <v>33.121000000000002</v>
       </c>
       <c r="C101">
-        <v>29.963999999999999</v>
+        <v>20.43</v>
       </c>
       <c r="D101">
         <v>40.152000000000001</v>
       </c>
       <c r="E101">
-        <v>20</v>
+        <v>33.090169940000003</v>
       </c>
       <c r="F101">
-        <v>30</v>
+        <v>20.489434840000001</v>
       </c>
       <c r="G101">
         <v>40</v>
@@ -6723,22 +7105,26 @@
       <c r="O101" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="T101">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B102">
-        <v>21.925000000000001</v>
+        <v>38.121000000000002</v>
       </c>
       <c r="C102">
-        <v>24.087</v>
+        <v>24.071000000000002</v>
       </c>
       <c r="D102">
         <v>40.152000000000001</v>
       </c>
       <c r="E102">
-        <v>21.909830060000001</v>
+        <v>38.090169940000003</v>
       </c>
       <c r="F102">
         <v>24.122147479999999</v>
@@ -6767,141 +7153,25 @@
       <c r="O102" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A103">
-        <v>98</v>
-      </c>
-      <c r="B103">
-        <v>26.931999999999999</v>
-      </c>
-      <c r="C103">
-        <v>20.437999999999999</v>
-      </c>
-      <c r="D103">
-        <v>40.152000000000001</v>
-      </c>
-      <c r="E103">
-        <v>26.909830060000001</v>
-      </c>
-      <c r="F103">
-        <v>20.489434840000001</v>
-      </c>
-      <c r="G103">
-        <v>40</v>
-      </c>
-      <c r="H103" t="s">
-        <v>98</v>
-      </c>
-      <c r="I103">
-        <v>7.7283896780000001</v>
-      </c>
-      <c r="J103">
-        <v>7.73638277602298</v>
-      </c>
-      <c r="K103" t="b">
-        <v>1</v>
-      </c>
-      <c r="M103">
-        <v>1</v>
-      </c>
-      <c r="N103">
-        <v>1</v>
-      </c>
-      <c r="O103" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A104">
-        <v>99</v>
-      </c>
-      <c r="B104">
-        <v>33.121000000000002</v>
-      </c>
-      <c r="C104">
-        <v>20.43</v>
-      </c>
-      <c r="D104">
-        <v>40.152000000000001</v>
-      </c>
-      <c r="E104">
-        <v>33.090169940000003</v>
-      </c>
-      <c r="F104">
-        <v>20.489434840000001</v>
-      </c>
-      <c r="G104">
-        <v>40</v>
-      </c>
-      <c r="H104" t="s">
-        <v>99</v>
-      </c>
-      <c r="I104">
-        <v>7.7283896780000001</v>
-      </c>
-      <c r="J104">
-        <v>7.73638277602298</v>
-      </c>
-      <c r="K104" t="b">
-        <v>1</v>
-      </c>
-      <c r="M104">
-        <v>1</v>
-      </c>
-      <c r="N104">
-        <v>1</v>
-      </c>
-      <c r="O104" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A105">
-        <v>100</v>
-      </c>
-      <c r="B105">
-        <v>38.121000000000002</v>
-      </c>
-      <c r="C105">
-        <v>24.071000000000002</v>
-      </c>
-      <c r="D105">
-        <v>40.152000000000001</v>
-      </c>
-      <c r="E105">
-        <v>38.090169940000003</v>
-      </c>
-      <c r="F105">
-        <v>24.122147479999999</v>
-      </c>
-      <c r="G105">
-        <v>40</v>
-      </c>
-      <c r="H105" t="s">
-        <v>100</v>
-      </c>
-      <c r="I105">
-        <v>7.7283896780000001</v>
-      </c>
-      <c r="J105">
-        <v>7.73638277602298</v>
-      </c>
-      <c r="K105" t="b">
-        <v>1</v>
-      </c>
-      <c r="M105">
-        <v>1</v>
-      </c>
-      <c r="N105">
-        <v>1</v>
-      </c>
-      <c r="O105" t="b">
-        <v>1</v>
+      <c r="T102">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T103">
+        <f>SUM(T2:T102)</f>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
     <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="R1:R2"/>
     <mergeCell ref="T1:T2"/>
@@ -6911,13 +7181,20 @@
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="P1:P2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
   </mergeCells>
+  <conditionalFormatting sqref="K3:K102">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O3:O45">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>